<commit_message>
Tuesday 16 July signoff backup
</commit_message>
<xml_diff>
--- a/GanttChart.xlsx
+++ b/GanttChart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\AVVR-Pipeline-Internship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44B7ABDB-349F-4B44-A69D-431866D694B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A1B95C-B94F-43DB-93B6-CE00CB57D553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Task</t>
   </si>
@@ -172,6 +172,18 @@
   </si>
   <si>
     <t>Updated TODO, focused on fixing git repo issues, added LFS, faced issues with remote branch separation, decided to create a new repo, dealt with submodules, forked all related submodules and made them public, faced authorization problems with Vscode, used GitHub Desktop instead, realized I committed weights by mistake, corrected by following ReadMe.md instructions, decided not to fork BoostingMonocularDepth as it's not used, added forked submodules properly with git submodule add, added gitignore for module weights/data, replaced AV-VR directory references, Phase 2 refactor ongoing to centralize main directory definition, committed changes multiple times, will test script functionality tomorrow.</t>
+  </si>
+  <si>
+    <t>Tested and confirmed GUI.py and Unity project work, focused on Steam Audio quirks, decided to create a fresh Steam Audio project for comparison, noted exact dimension reproduction for monodepth isn't crucial, explored enhance360.py arguments to strengthen depth maps without complex preprocessing, found increasing baseline value helps retain detail, faced issues at baseline 5.264, followed digital audio fundamentals on YouTube, planning to use Audacity for waveform comparison, considered simplifying preprocessing by removing top and bottom modifications only, realized mirror fixes were incidental, commented out plane detection in enhance360.py for better results, but still need to address some depth loss.</t>
+  </si>
+  <si>
+    <t>Worked from home, cleaned up the GitHub repo for better pulls, faced issues with Unity project .meta files and prefab initialization, ran into Git LFS bandwidth limits due to repeated .obj file pulls, decided to check for .obj file existence before import to avoid errors, planned to use a different storage provider for large files, decided to update the manual with a basic checklist for new PC/system setups, considered reactivating boostingMonocularDepth in 360monodepth for better depth images without enhance360.py, updated TODO to include fixing Steam Audio quirks, optimizing monodepth with boostingMonocularDepth, and removing Docker clutter.</t>
+  </si>
+  <si>
+    <t>Met with Dr. Hansung Kim at 10:30 am, discussed improving Unity project realism, adding collision for non-VR player controller, implementing binaural audio, and checking RIR calculations. Mona will WFH next week; asked necessary questions and to send recording to Dr. Hansung for feedback. Updated  Fixed Dockerfile build error, confirmed Monodepth v1.0 has different Image IDs, refactored code, compared enhance360.py with new enhance360mono.py, found enhance360mono better for depth details but less accurate for room structure. Tested on UL, found MonodepthBoosting not as good as manual edge optimization, generated meshes showed artifacts, MR scene better but not ideal. Plan to generate all scenes and consult Dr. Hansung Kim, identified V2's white balance issue, will figure out monoenhance tomorrow, and may fallback to enhance360.py baseline 2.264.</t>
+  </si>
+  <si>
+    <t>Reconfigured StartScene to include Steam Audio Probe Batch, added baked source and listener components, changed behavior to baked as per Mona’s recommendation, exported audio using Wavepad or Audacity, added checks and dynamic project directory, confirmed settings with Mona’s suggestions. Found baked settings clearer in directivity and reverb compared to real-time, note to export active scenes after every bake. Encountered bug with old project directory, fixed by reimporting Steam Audio. Baked probe only has one level when using uniform floor mode, requiring player controller with collision for realism. Radeon Rays mode caused OpenCL error, unsure about TrueNext in reflection mode. Baking time should be minimal if correctly configured. Experienced bug with occlusion and distance attenuation in freecam mode. Decided to have an in-game indicator for Steam Audio status. Shifted focus to enhance360mono, created visualizer script, identified fix limits as the issue, promising results with fix_limits_mono from Claude. Signed off for the day.</t>
   </si>
 </sst>
 </file>
@@ -516,7 +528,7 @@
   <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -636,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8289DD30-5B10-44EC-835E-469611DFB1F9}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -717,23 +729,35 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="261" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>43</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="319" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
         <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Wednesday 17 July signoff backup
</commit_message>
<xml_diff>
--- a/GanttChart.xlsx
+++ b/GanttChart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\AVVR-Pipeline-Internship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A1B95C-B94F-43DB-93B6-CE00CB57D553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A15E77-33B6-4698-AC09-F387BE99E578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Task</t>
   </si>
@@ -184,6 +184,9 @@
   </si>
   <si>
     <t>Reconfigured StartScene to include Steam Audio Probe Batch, added baked source and listener components, changed behavior to baked as per Mona’s recommendation, exported audio using Wavepad or Audacity, added checks and dynamic project directory, confirmed settings with Mona’s suggestions. Found baked settings clearer in directivity and reverb compared to real-time, note to export active scenes after every bake. Encountered bug with old project directory, fixed by reimporting Steam Audio. Baked probe only has one level when using uniform floor mode, requiring player controller with collision for realism. Radeon Rays mode caused OpenCL error, unsure about TrueNext in reflection mode. Baking time should be minimal if correctly configured. Experienced bug with occlusion and distance attenuation in freecam mode. Decided to have an in-game indicator for Steam Audio status. Shifted focus to enhance360mono, created visualizer script, identified fix limits as the issue, promising results with fix_limits_mono from Claude. Signed off for the day.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Received MATLAB and Python code for audio evaluation from Mona, reviewed GDP’s KT LS1/LS2 position images and old S3A unity project for correct cam/listener and audio source positions, standardized scene sizes in meters for setup. Need to confirm Steam Audio settings with Mona and reconfigured the project directory. Created helper scripts/gameobjects for dimension calculation, centering, and scaling of imported models. Adjusted coordinates and scaling ratios for accurate positioning. Fixed bugs and ensured functionality of AudioCameraPositioner editor menu helper script. </t>
   </si>
 </sst>
 </file>
@@ -231,7 +234,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -244,6 +247,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -759,6 +765,9 @@
       <c r="C5" s="2" t="s">
         <v>48</v>
       </c>
+      <c r="D5" s="7" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="6">

</xml_diff>

<commit_message>
Friday 19 July signoff, regenerated daily log summary using claude instead because chatgpt sucks
Former-commit-id: bd4bf0490e7905903b35d865d7a46dd2736cf665
</commit_message>
<xml_diff>
--- a/GanttChart.xlsx
+++ b/GanttChart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\AVVR-Pipeline-Internship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A15E77-33B6-4698-AC09-F387BE99E578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4330ECA6-C855-48B2-8A92-F46D4A7C32F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Task</t>
   </si>
@@ -144,49 +144,55 @@
     <t>Weekly Notes</t>
   </si>
   <si>
-    <t>Fixed 360monodepth directory refs, Edgenet360 fixes: switched to anaconda, updated install steps, fixed TensorFlow ValueError, added checks for IndexError, generated/compared smoothed vs. unsmoothed meshes, fixed UnboundLocalError in Meeting Room scene, forked Edgenet360 to my GitHub, pushed changes.</t>
-  </si>
-  <si>
     <t>Starting week 2, there's also .docx log in AV-VR-Internship/Intern-Logs folder for each week work, so refer those for more details</t>
   </si>
   <si>
-    <t>Prepped for meeting, cleaned GitHub repo, refactored smoothing index error fix, generated 5 scene meshes (KT, LR, MR, ST, UL) and intermediary outputs, tested importing meshes into Unity, used keyboardmove.cs for non-VR testing, noted sound differences, occlusion issues, need to remove anomaly meshes, meeting with Dr. Hansung Kim: advised to keep reading and work on mesh cleanup, updated, modified GUI.py to render without ceiling, regenerated and committed all meshes. TODO: clean up meshes (top and bottom camera occlusion)</t>
-  </si>
-  <si>
-    <t>Thought about optimal solution, remove anomalies early in pipeline or post mesh generation, noted voxel anomalies linked to floor/ceiling, considered radius-based removal around origin, tested in Blender, found excessive vertices, realized material links missing in Blender, discussed with Mona about enhance360 for depth map, added enhance360.py to pipeline, fixed cone anomaly in meshes, found include_top parameter not working, updated TODOs, learned to verify tools thoroughly, found dynamic height cutoff working for ceiling removal in KT and LR.</t>
-  </si>
-  <si>
     <t>This wont just stop at Week 1, but the 3 most important papers emailed to me had been finished read by then</t>
   </si>
   <si>
-    <t>Generated scene meshes, noted Docker desktop dependency, MR ceiling material issue fixed by shifting, inconsistent output observed, ST scene correct, proposed pipeline automation for shifting, ceiling removal note, Edgenet360 paper insights on enhance360, compromise in detail loss with enhanced depth maps, UL depth map issue noted, adjusted ceiling cutoff. Shifting improves MR material assignment but needs a stronger depth map. Explore enhance360 and monodepth parameter tweaks. Future work: add more sound options for better UX/UI.</t>
-  </si>
-  <si>
-    <t>WFH, not much done again. Read papers and tried pulling repo to personal PC. Didn't work yet as missing submodules properly and need git LFS for LiDaR for Unity to work, or exclude the import in the script.</t>
-  </si>
-  <si>
-    <t>Material assignment inconsistency in UL, add pre-enhancement step for depth map, ensure room dimensions match ground truth or stereo depth map, dimension comparison (HxWxL) for MR, KT, LR, ST, UL, different from ground truth and stereo depth map, KT scaling issue, fits LiDAR scan best, need Dr. Hansung Kim's clarification, experiment with preprocessing steps for better visual results, UL Kim21 import issues in Unity, broken normal map? MR rgb actually already shifted, its height slightly shorter, pipeline lacks object details in final mesh, hinders evaluation, material recognition issues due to cubemap projection limitation, weird filepath error in main GUI.py pipeline, debug tomorrow.</t>
-  </si>
-  <si>
-    <t>refactored combined.bat to be more modular, fixed bugs, 3rd meeting w/ Dr Hansung Kim, discussed correct dimension scaling, Steam Audio issues, mesh optimization, obtained audio eval code from Mona, tried making monodepth depth map stronger, worked on modular pipeline refactor, fixed pipeline bugs, encountered issues with .jpg and .png files, fixed shifting bugs, tested Steam Audio settings, accessed Steam Audio docs via Wayback Machine, resolved broken pipeline issues, fixed directory path errors, confirmed KT without ceiling works, tested and confirmed MR with ceiling works, need further refactoring for hardcoded directories and temp output removal, Phase 1 refactor complete.</t>
-  </si>
-  <si>
-    <t>Updated TODO, focused on fixing git repo issues, added LFS, faced issues with remote branch separation, decided to create a new repo, dealt with submodules, forked all related submodules and made them public, faced authorization problems with Vscode, used GitHub Desktop instead, realized I committed weights by mistake, corrected by following ReadMe.md instructions, decided not to fork BoostingMonocularDepth as it's not used, added forked submodules properly with git submodule add, added gitignore for module weights/data, replaced AV-VR directory references, Phase 2 refactor ongoing to centralize main directory definition, committed changes multiple times, will test script functionality tomorrow.</t>
-  </si>
-  <si>
-    <t>Tested and confirmed GUI.py and Unity project work, focused on Steam Audio quirks, decided to create a fresh Steam Audio project for comparison, noted exact dimension reproduction for monodepth isn't crucial, explored enhance360.py arguments to strengthen depth maps without complex preprocessing, found increasing baseline value helps retain detail, faced issues at baseline 5.264, followed digital audio fundamentals on YouTube, planning to use Audacity for waveform comparison, considered simplifying preprocessing by removing top and bottom modifications only, realized mirror fixes were incidental, commented out plane detection in enhance360.py for better results, but still need to address some depth loss.</t>
-  </si>
-  <si>
-    <t>Worked from home, cleaned up the GitHub repo for better pulls, faced issues with Unity project .meta files and prefab initialization, ran into Git LFS bandwidth limits due to repeated .obj file pulls, decided to check for .obj file existence before import to avoid errors, planned to use a different storage provider for large files, decided to update the manual with a basic checklist for new PC/system setups, considered reactivating boostingMonocularDepth in 360monodepth for better depth images without enhance360.py, updated TODO to include fixing Steam Audio quirks, optimizing monodepth with boostingMonocularDepth, and removing Docker clutter.</t>
-  </si>
-  <si>
-    <t>Met with Dr. Hansung Kim at 10:30 am, discussed improving Unity project realism, adding collision for non-VR player controller, implementing binaural audio, and checking RIR calculations. Mona will WFH next week; asked necessary questions and to send recording to Dr. Hansung for feedback. Updated  Fixed Dockerfile build error, confirmed Monodepth v1.0 has different Image IDs, refactored code, compared enhance360.py with new enhance360mono.py, found enhance360mono better for depth details but less accurate for room structure. Tested on UL, found MonodepthBoosting not as good as manual edge optimization, generated meshes showed artifacts, MR scene better but not ideal. Plan to generate all scenes and consult Dr. Hansung Kim, identified V2's white balance issue, will figure out monoenhance tomorrow, and may fallback to enhance360.py baseline 2.264.</t>
-  </si>
-  <si>
-    <t>Reconfigured StartScene to include Steam Audio Probe Batch, added baked source and listener components, changed behavior to baked as per Mona’s recommendation, exported audio using Wavepad or Audacity, added checks and dynamic project directory, confirmed settings with Mona’s suggestions. Found baked settings clearer in directivity and reverb compared to real-time, note to export active scenes after every bake. Encountered bug with old project directory, fixed by reimporting Steam Audio. Baked probe only has one level when using uniform floor mode, requiring player controller with collision for realism. Radeon Rays mode caused OpenCL error, unsure about TrueNext in reflection mode. Baking time should be minimal if correctly configured. Experienced bug with occlusion and distance attenuation in freecam mode. Decided to have an in-game indicator for Steam Audio status. Shifted focus to enhance360mono, created visualizer script, identified fix limits as the issue, promising results with fix_limits_mono from Claude. Signed off for the day.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Received MATLAB and Python code for audio evaluation from Mona, reviewed GDP’s KT LS1/LS2 position images and old S3A unity project for correct cam/listener and audio source positions, standardized scene sizes in meters for setup. Need to confirm Steam Audio settings with Mona and reconfigured the project directory. Created helper scripts/gameobjects for dimension calculation, centering, and scaling of imported models. Adjusted coordinates and scaling ratios for accurate positioning. Fixed bugs and ensured functionality of AudioCameraPositioner editor menu helper script. </t>
+    <t>Organized Unity project folders. Investigated ModelDimension calculation issue. Tested .obj/.mtl import. Explored edgenet library limitations. Noted ST model scaling in Unity. Updated .gitignore. Planned to publish Internship-tools repo.</t>
+  </si>
+  <si>
+    <t>Updated .gitignore. Investigated Steam Audio settings. Discovered Mesh Dimension Calculator bug. Generated and aligned 5 evaluation scenes. Set up audio sources per S3A settings. Filled dimension table. Established audio baking/export workflow.</t>
+  </si>
+  <si>
+    <t>Received MATLAB/Python audio evaluation code. Created helper scripts for model dimension calculation and positioning. Debugged and improved AudioCameraPositioner editor menu. Standardized scene scaling and alignment for 5 evaluation scenes. Updated TODO list.</t>
+  </si>
+  <si>
+    <t>Reconfigured StartScene with Steam Audio components. Fixed project directory issues. Debugged Steam Audio settings and baking process. Created visualizer script for enhance360.py. Improved fix_limits_mono function for depth map enhancement.</t>
+  </si>
+  <si>
+    <t>4th meeting with Dr. Kim. Updated TODO list. Fixed Dockerfile build error. Tested BoostingMonocularDepth vs original enhance360.py. Compared depth maps and generated meshes for different scenes. Identified issues with mono depth enhancement.</t>
+  </si>
+  <si>
+    <t>Reviewed TODO list. Investigated depth map enhancement for monodepth. Compared room dimensions from different methods. Analyzed mesh quality and material recognition issues. Encountered pipeline error in GUI.py.</t>
+  </si>
+  <si>
+    <t>3rd meeting with Dr. Kim. Updated TODO list. Refactored pipeline for modularity. Debugged file path issues. Investigated Steam Audio settings. Successfully tested KT and MR scenes. Planned further refactoring and optimization.</t>
+  </si>
+  <si>
+    <t>Updated TODO list. Created new repo to fix git issues. Forked and added submodules. Updated .gitignore for weights/data. Started Phase 2 refactoring to centralize project directory definition.</t>
+  </si>
+  <si>
+    <t>Tested GUI.py functionality. Explored Steam Audio settings. Experimented with monodepth optimization, focusing on baseline adjustments. Started audio fundamentals study. Simplified depth map enhancement process, focusing on ceiling/floor modification.</t>
+  </si>
+  <si>
+    <t>WFH. Addressed Unity project issues. Encountered Git LFS bandwidth limit. Updated manual for setup process. Identified potential fix for monodepth optimization using boostingMonocularDepth. Updated TODO list.</t>
+  </si>
+  <si>
+    <t>Fixed 360monodepth directory issues. Resolved Edgenet360 errors (miniconda, TensorFlow, smoothing). Generated meshes for all scenes. Fixed UnboundLocalError in file_utils.py. Forked and updated Edgenet360/Mesh-generation repo. Planned to rerun and organize outputs.</t>
+  </si>
+  <si>
+    <t>2nd meeting with Dr. Kim. Cleaned GitHub repo. Refactored smoothing fix. Generated and imported 5 scene meshes into Unity. Tested audio in VR/non-VR modes. Identified mesh anomalies. Updated TODO list. Regenerated scene meshes with all .obj outputs.</t>
+  </si>
+  <si>
+    <t>Solved mesh anomaly issue by implementing enhance360.py step. Updated pipeline and GUI.py. Fixed --include-top parameter bug. Explored dynamic ceiling removal methods. Updated TODO list. Tested new mesh generation process on KT and LR scenes.</t>
+  </si>
+  <si>
+    <t>Added image shifting option to pipeline. Regenerated all scene meshes with/without ceilings. Investigated depth map enhancement issues. Fixed material assignment bug. Updated TODO list. Explored options for improving monodepth output for enhance360 compatibility.</t>
+  </si>
+  <si>
+    <t>WFH. Read papers. Tested repo pull. Identified issues with submodules and Git LFS. Found ML pipeline broken due to missing submodules. Noted repo size issues (8GB). Planned to remove bloat and fix submodule/LFS problems.</t>
   </si>
 </sst>
 </file>
@@ -534,7 +540,7 @@
   <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -605,7 +611,7 @@
       </c>
       <c r="B3" s="1"/>
       <c r="N3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.35">
@@ -654,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8289DD30-5B10-44EC-835E-469611DFB1F9}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -692,7 +698,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="102" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="116" x14ac:dyDescent="0.35">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -712,30 +718,30 @@
         <v>33</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="172" customHeight="1" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>38</v>
+        <v>47</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="261" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -748,25 +754,31 @@
       <c r="D4" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="3" t="s">
         <v>45</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="319" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>48</v>
+        <v>41</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>49</v>
+        <v>39</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Monday 23 July signoff backup
</commit_message>
<xml_diff>
--- a/GanttChart.xlsx
+++ b/GanttChart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\AVVR-Pipeline-Internship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4330ECA6-C855-48B2-8A92-F46D4A7C32F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1DB0EF-1DCC-49F5-8222-9BA34C791198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Task</t>
   </si>
@@ -193,6 +193,9 @@
   </si>
   <si>
     <t>WFH. Read papers. Tested repo pull. Identified issues with submodules and Git LFS. Found ML pipeline broken due to missing submodules. Noted repo size issues (8GB). Planned to remove bloat and fix submodule/LFS problems.</t>
+  </si>
+  <si>
+    <t>Attended Midway Development Day talks. Updated TODO list. Set up audio recording process for evaluation scenes using Audacity and Sony WH1000-XM4 headphones. Adjusted Matlab code for octave band analysis. Prepared RIR file extraction process using Mona's .ipynb code.</t>
   </si>
 </sst>
 </file>
@@ -661,7 +664,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -781,9 +784,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
analysed converted 44.1kHz MR sweep (RT60 correct, EDT problematic)
Former-commit-id: ad42d7eb5ac15d6c101e287280503680195c88f3
</commit_message>
<xml_diff>
--- a/GanttChart.xlsx
+++ b/GanttChart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\AVVR-Pipeline-Internship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1DB0EF-1DCC-49F5-8222-9BA34C791198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B53FBFF-B0C6-4FF1-85CE-23E7CF041FB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="10 Week" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>Task</t>
   </si>
@@ -196,6 +196,21 @@
   </si>
   <si>
     <t>Attended Midway Development Day talks. Updated TODO list. Set up audio recording process for evaluation scenes using Audacity and Sony WH1000-XM4 headphones. Adjusted Matlab code for octave band analysis. Prepared RIR file extraction process using Mona's .ipynb code.</t>
+  </si>
+  <si>
+    <t>Generated all audio. Organized RIR analysis folders. Modified MATLAB scripts for compatibility. Investigated and troubleshooted EDT/RT60 analysis issues. Experimented with different audio settings (sampling rate, sine sweep type, probe number, audio delay, volume). Identified persistent problems with audio analysis results.</t>
+  </si>
+  <si>
+    <t>Gonna go longer than week 4, hopefully finish analysis with pretty graphs etc by end of Week 5</t>
+  </si>
+  <si>
+    <t>Extended</t>
+  </si>
+  <si>
+    <t>Cancelled/Delayed</t>
+  </si>
+  <si>
+    <t>This is now optional, SSC Mona is using stereo (some problem/setback?)</t>
   </si>
 </sst>
 </file>
@@ -211,7 +226,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -230,6 +245,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -243,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -260,6 +287,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q8"/>
+  <dimension ref="A1:V8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -551,7 +580,7 @@
     <col min="1" max="1" width="30.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -566,8 +595,16 @@
         <v>26</v>
       </c>
       <c r="Q1" s="5"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S1" s="8"/>
+      <c r="T1" t="s">
+        <v>56</v>
+      </c>
+      <c r="V1" s="9"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -608,47 +645,54 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="5"/>
       <c r="N3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="4"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>22</v>
       </c>
       <c r="C5" s="4"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="8"/>
+      <c r="N5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="1"/>
+      <c r="F6" s="9"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="N6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>27</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -663,8 +707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8289DD30-5B10-44EC-835E-469611DFB1F9}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -784,12 +828,15 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>52</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
tested S3A setting with Mona volume and distance attenuation parameter (it does matter)
Former-commit-id: d6b4caba4ef080441984278a484f1f305bb7c1ea
</commit_message>
<xml_diff>
--- a/GanttChart.xlsx
+++ b/GanttChart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\AVVR-Pipeline-Internship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B53FBFF-B0C6-4FF1-85CE-23E7CF041FB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{296FCBA5-9ACE-4898-B4FE-35CFFB271FDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="10 Week" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>Task</t>
   </si>
@@ -211,6 +211,10 @@
   </si>
   <si>
     <t>This is now optional, SSC Mona is using stereo (some problem/setback?)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Met with Dr. Kim. Reviewed progress and plans. Investigated EDT/RT60 analysis issues. Discovered audio cutoff bug related to Steam Audio initialization. Experimented with various audio settings and recording methods. Identified potential causes for high EDT values. Continued troubleshooting audio analysis discrepancies.
+</t>
   </si>
 </sst>
 </file>
@@ -270,7 +274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -289,6 +293,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,7 +578,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
@@ -707,8 +714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8289DD30-5B10-44EC-835E-469611DFB1F9}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -828,15 +835,18 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="116" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>53</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
recovered updated logs from backup and removed no longer used convertlfs script
</commit_message>
<xml_diff>
--- a/GanttChart.xlsx
+++ b/GanttChart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\AVVR-Pipeline-Internship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{296FCBA5-9ACE-4898-B4FE-35CFFB271FDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4425D443-D000-4641-84C6-BB33A2F234FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>Task</t>
   </si>
@@ -215,6 +215,9 @@
   <si>
     <t xml:space="preserve"> Met with Dr. Kim. Reviewed progress and plans. Investigated EDT/RT60 analysis issues. Discovered audio cutoff bug related to Steam Audio initialization. Experimented with various audio settings and recording methods. Identified potential causes for high EDT values. Continued troubleshooting audio analysis discrepancies.
 </t>
+  </si>
+  <si>
+    <t>Conducted extensive testing of audio settings across different scenes (KT, MR, ST). Investigated causes of high EDT and RT60 values. Experimented with various mix ratios, volume levels, and Steam Audio parameters. Identified physics-based attenuation as beneficial. Concluded to use Mona's settings with modifications: physics-based attenuation, air absorption, 0.5 volume, and RT60 from extrapolated RT30. Noted limitations in Unity Steam Audio simulation for accurate EDT reproduction.</t>
   </si>
 </sst>
 </file>
@@ -274,7 +277,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -293,9 +296,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -714,8 +714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8289DD30-5B10-44EC-835E-469611DFB1F9}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -835,7 +835,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="116" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="174" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -845,8 +845,11 @@
       <c r="C6" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="7" t="s">
         <v>58</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Monday 30 Jul signoff backup
</commit_message>
<xml_diff>
--- a/GanttChart.xlsx
+++ b/GanttChart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\AVVR-Pipeline-Internship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4425D443-D000-4641-84C6-BB33A2F234FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2300A05-AEB8-4989-A696-33026B341D1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="10 Week" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>Task</t>
   </si>
@@ -218,6 +218,15 @@
   </si>
   <si>
     <t>Conducted extensive testing of audio settings across different scenes (KT, MR, ST). Investigated causes of high EDT and RT60 values. Experimented with various mix ratios, volume levels, and Steam Audio parameters. Identified physics-based attenuation as beneficial. Concluded to use Mona's settings with modifications: physics-based attenuation, air absorption, 0.5 volume, and RT60 from extrapolated RT30. Noted limitations in Unity Steam Audio simulation for accurate EDT reproduction.</t>
+  </si>
+  <si>
+    <t>Week 5 Friday: Resolved Git LFS issues by uninstalling LFS and restructuring repository. Attempted to implement RT30 for RT60 estimation. Encountered difficulties with irStats function parameter adjustments. Experimented with various approaches but faced persistent calculation issues.</t>
+  </si>
+  <si>
+    <t>Investigated RT30 calculation issues. Discovered limitations in energy decay curve fitting. Revised focus to troubleshoot RT60 problems in Unity. Experimented with various Unity/Steam Audio settings to reduce noise floor level. Tested different volume levels, mix ratios, and HRTF settings. Planned comprehensive review of all related components and settings for further troubleshooting.</t>
+  </si>
+  <si>
+    <t>WFH. Conducted in-depth review of MATLAB code. Researched related topics to enhance understanding of audio analysis and room acoustics. Prepared for further troubleshooting based on new insights.</t>
   </si>
 </sst>
 </file>
@@ -714,8 +723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8289DD30-5B10-44EC-835E-469611DFB1F9}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -851,10 +860,19 @@
       <c r="E6" s="7" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F6" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>6</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
gantt chart update and papers added
</commit_message>
<xml_diff>
--- a/GanttChart.xlsx
+++ b/GanttChart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\AVVR-Pipeline-Internship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2300A05-AEB8-4989-A696-33026B341D1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F24FA0-829E-461E-8EB4-2A5C9AC63A7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>Task</t>
   </si>
@@ -227,6 +227,12 @@
   </si>
   <si>
     <t>WFH. Conducted in-depth review of MATLAB code. Researched related topics to enhance understanding of audio analysis and room acoustics. Prepared for further troubleshooting based on new insights.</t>
+  </si>
+  <si>
+    <t>Identified critical bug in irStats MATLAB function. Found hardcoded values preventing proper y_fit parameter usage. Tested various RT calculations (RT20, RT25, RT30) on ST scene. Determined RT25 as optimal middle ground. Planned dynamic value adjustment based on y_fit argument for tomorrow.</t>
+  </si>
+  <si>
+    <t>Modified irStats.m for dynamic value range. Tested various RT calculations across scenes. Identified inconsistencies in EDT and RT60 calculations. Investigated Kim21 and Mona's results. Discovered pre-existing audio files for reference. Revised plan to focus on investigating other MATLAB scripts, verifying older methods, and replicating results with current scenes.</t>
   </si>
 </sst>
 </file>
@@ -724,7 +730,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -874,26 +880,53 @@
       <c r="C7" s="3" t="s">
         <v>62</v>
       </c>
+      <c r="D7" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
         <v>7</v>
       </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
         <v>8</v>
       </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="6">
         <v>9</v>
       </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <v>10</v>
       </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
reanalysed KT,MR, and LR
</commit_message>
<xml_diff>
--- a/GanttChart.xlsx
+++ b/GanttChart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\AVVR-Pipeline-Internship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F24FA0-829E-461E-8EB4-2A5C9AC63A7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CBDF4CC-FAA0-4FF2-9F83-2CD0D225A2E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>Task</t>
   </si>
@@ -233,6 +233,9 @@
   </si>
   <si>
     <t>Modified irStats.m for dynamic value range. Tested various RT calculations across scenes. Identified inconsistencies in EDT and RT60 calculations. Investigated Kim21 and Mona's results. Discovered pre-existing audio files for reference. Revised plan to focus on investigating other MATLAB scripts, verifying older methods, and replicating results with current scenes.</t>
+  </si>
+  <si>
+    <t>Investigated plotting_rir_compare.m script. Determined older scripts less relevant for current needs. Focused on generating results for each scene. Tuned parameters individually for KT, LR, and MR scenes. Observed persistent issues with noise floor levels and frequency-dependent RT calculations. Planned to complete ST and UL scene analysis next week.</t>
   </si>
 </sst>
 </file>
@@ -730,7 +733,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -870,7 +873,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="145" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -886,7 +889,9 @@
       <c r="E7" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="F7" s="3"/>
+      <c r="F7" s="3" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="6">

</xml_diff>

<commit_message>
Monday 5 August verdict and analysis
</commit_message>
<xml_diff>
--- a/GanttChart.xlsx
+++ b/GanttChart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\AVVR-Pipeline-Internship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CBDF4CC-FAA0-4FF2-9F83-2CD0D225A2E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31326B5D-2092-4319-9DCB-8F66BB5C2012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
     <t>Task</t>
   </si>
@@ -236,6 +236,9 @@
   </si>
   <si>
     <t>Investigated plotting_rir_compare.m script. Determined older scripts less relevant for current needs. Focused on generating results for each scene. Tuned parameters individually for KT, LR, and MR scenes. Observed persistent issues with noise floor levels and frequency-dependent RT calculations. Planned to complete ST and UL scene analysis next week.</t>
+  </si>
+  <si>
+    <t>Refined result presentation for easier comparison with Kim21. Created separate scripts for each scene. Reverted irStats.m changes after realizing misunderstanding. Generated new results (v2) for all scenes with adjusted parameters. Observed inconsistencies across octave bands compared to Kim21. Analyzed Mona's latest audio results. Theorized potential limitations in recording method or audio source (sine sweep) as cause for discrepancies.</t>
   </si>
 </sst>
 </file>
@@ -732,7 +735,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8289DD30-5B10-44EC-835E-469611DFB1F9}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -893,11 +896,13 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="145" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
         <v>7</v>
       </c>
-      <c r="B8" s="3"/>
+      <c r="B8" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>

</xml_diff>

<commit_message>
Added basic audio recording through unity (still buggy)
</commit_message>
<xml_diff>
--- a/GanttChart.xlsx
+++ b/GanttChart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\AVVR-Pipeline-Internship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31326B5D-2092-4319-9DCB-8F66BB5C2012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F01C20C4-E5E3-480A-8CDE-3BCBAEA4913E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="10 Week" sheetId="1" r:id="rId1"/>
@@ -736,7 +736,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Wednesday 7 August trial and error
</commit_message>
<xml_diff>
--- a/GanttChart.xlsx
+++ b/GanttChart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\AVVR-Pipeline-Internship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F01C20C4-E5E3-480A-8CDE-3BCBAEA4913E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{460FD502-4FAC-4EF4-BDB1-ED723668F612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>Task</t>
   </si>
@@ -239,6 +239,12 @@
   </si>
   <si>
     <t>Refined result presentation for easier comparison with Kim21. Created separate scripts for each scene. Reverted irStats.m changes after realizing misunderstanding. Generated new results (v2) for all scenes with adjusted parameters. Observed inconsistencies across octave bands compared to Kim21. Analyzed Mona's latest audio results. Theorized potential limitations in recording method or audio source (sine sweep) as cause for discrepancies.</t>
+  </si>
+  <si>
+    <t>Met with Dr. Hansung Kim. Discussed ongoing audio analysis issues. Confirmed project details (ceiling inclusion, audio recording method). Implemented direct audio capture in Unity. Created AudioCapture.cs and AudioRecorder.cs scripts. Successfully fixed 4-second audio cutoff issue. Planned to test new recording method on sine sweep for RIR tomorrow.</t>
+  </si>
+  <si>
+    <t>Successfully tested direct Unity audio recording without headphones. Experimented with various volume levels (0.1 to 1.0) to prevent clipping in KT scene. Adjusted mix levels for direct and reflected sound. Planned to test gunshot and different sine sweep signals. Decided to rewrite parts of analysis .ipynb for new audio sources.</t>
   </si>
 </sst>
 </file>
@@ -736,7 +742,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -903,8 +909,12 @@
       <c r="B8" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+      <c r="C8" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>

</xml_diff>

<commit_message>
updated gantt chart daily logs
</commit_message>
<xml_diff>
--- a/GanttChart.xlsx
+++ b/GanttChart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\AVVR-Pipeline-Internship\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\AVVR-Pipeline-Internship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{460FD502-4FAC-4EF4-BDB1-ED723668F612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC7F931D-C26B-4FB1-992F-8EDBF4CBDC53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="10 Week" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>Task</t>
   </si>
@@ -245,6 +245,12 @@
   </si>
   <si>
     <t>Successfully tested direct Unity audio recording without headphones. Experimented with various volume levels (0.1 to 1.0) to prevent clipping in KT scene. Adjusted mix levels for direct and reflected sound. Planned to test gunshot and different sine sweep signals. Decided to rewrite parts of analysis .ipynb for new audio sources.</t>
+  </si>
+  <si>
+    <t>WFH. Conducted research on sine sweep RIR methods. Studied video resources on room acoustics, acoustic measurements, and sine sweep optimization for room impulse response measurements.</t>
+  </si>
+  <si>
+    <t>Rewrote RIR_Analysis code for new sine sweep signals. Created improved sine sweep generation and deconvolve code in Jupyter notebook. Experimented with various mix ratios and volumes to address clipping and RT60 issues. Observed improvements in octave band responses but encountered persistent challenges with frequency-dependent RT60 values. Considered manual correction for each octave band and explored using smaller y_fit values like RT30.</t>
   </si>
 </sst>
 </file>
@@ -609,12 +615,12 @@
       <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -638,7 +644,7 @@
       </c>
       <c r="V1" s="9"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -679,7 +685,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -688,7 +694,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -696,7 +702,7 @@
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -708,7 +714,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -719,14 +725,14 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -741,22 +747,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8289DD30-5B10-44EC-835E-469611DFB1F9}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="6"/>
-    <col min="2" max="2" width="45.08984375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="46.6328125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="45.08984375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="42.54296875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="35.6328125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="22.08984375" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" style="6"/>
+    <col min="2" max="2" width="45.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="46.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="45.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="42.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="35.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>13</v>
       </c>
@@ -779,7 +785,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="116" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -802,7 +808,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -822,7 +828,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -842,7 +848,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -862,7 +868,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="174" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="180" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -882,7 +888,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="145" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -902,7 +908,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="145" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="195" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -915,10 +921,14 @@
       <c r="D8" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E8" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -928,7 +938,7 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -938,7 +948,7 @@
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
12 August daily log signoff
</commit_message>
<xml_diff>
--- a/GanttChart.xlsx
+++ b/GanttChart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\AVVR-Pipeline-Internship\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\AVVR-Pipeline-Internship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC7F931D-C26B-4FB1-992F-8EDBF4CBDC53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{446DA5D3-D70D-4AA4-8863-E0A3A0C7966B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="10 Week" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>Task</t>
   </si>
@@ -251,6 +251,9 @@
   </si>
   <si>
     <t>Rewrote RIR_Analysis code for new sine sweep signals. Created improved sine sweep generation and deconvolve code in Jupyter notebook. Experimented with various mix ratios and volumes to address clipping and RT60 issues. Observed improvements in octave band responses but encountered persistent challenges with frequency-dependent RT60 values. Considered manual correction for each octave band and explored using smaller y_fit values like RT30.</t>
+  </si>
+  <si>
+    <t>Reviewed last week's results. Tested various volume levels and mix ratios for KT scene. Improved sine sweep signal with longer duration (15 sec). Observed significant improvements in RT60 and EDT measurements. Identified remaining issues: pre-0s RIR distortion and frequency-dependent RT60 discrepancies. Planned further sine sweep optimization for tomorrow.</t>
   </si>
 </sst>
 </file>
@@ -615,12 +618,12 @@
       <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -644,7 +647,7 @@
       </c>
       <c r="V1" s="9"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -685,7 +688,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -694,7 +697,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -702,7 +705,7 @@
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -714,7 +717,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -725,14 +728,14 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>27</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -748,21 +751,21 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="6"/>
-    <col min="2" max="2" width="45.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="46.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="45.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="42.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="35.5703125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="8.7265625" style="6"/>
+    <col min="2" max="2" width="45.1796875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="46.54296875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="45.1796875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="42.54296875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="35.54296875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="22.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>13</v>
       </c>
@@ -785,7 +788,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="116" x14ac:dyDescent="0.35">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -808,7 +811,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -828,7 +831,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -848,7 +851,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -868,7 +871,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="174" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -888,7 +891,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="145" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -908,7 +911,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="195" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -928,17 +931,19 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="116" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
         <v>8</v>
       </c>
-      <c r="B9" s="3"/>
+      <c r="B9" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -948,7 +953,7 @@
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
tested GDP's sweep audio (interesting, require more testing)
</commit_message>
<xml_diff>
--- a/GanttChart.xlsx
+++ b/GanttChart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\AVVR-Pipeline-Internship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{446DA5D3-D70D-4AA4-8863-E0A3A0C7966B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29DF4013-242A-4DD7-AC3B-F17C03F42D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t>Task</t>
   </si>
@@ -254,6 +254,9 @@
   </si>
   <si>
     <t>Reviewed last week's results. Tested various volume levels and mix ratios for KT scene. Improved sine sweep signal with longer duration (15 sec). Observed significant improvements in RT60 and EDT measurements. Identified remaining issues: pre-0s RIR distortion and frequency-dependent RT60 discrepancies. Planned further sine sweep optimization for tomorrow.</t>
+  </si>
+  <si>
+    <t>Tested improved sine sweep v3 with longer duration and extended frequency range. Observed unexpected results. Reverted to v2 and disabled HRTF for mono RIR measurement. Rewrote main_KT Jupyter notebook for modularity. Tested original GDP sweep.wav, noting consistent but low RT60 values. Planned to explore audio source parameter tuning and prepare questions for Dr. Atiyeh.</t>
   </si>
 </sst>
 </file>
@@ -751,7 +754,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -938,7 +941,9 @@
       <c r="B9" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C9" s="3"/>
+      <c r="C9" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>

</xml_diff>

<commit_message>
tested no floor (weird anomaly behaviour, 2nd peak after first)
</commit_message>
<xml_diff>
--- a/GanttChart.xlsx
+++ b/GanttChart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\AVVR-Pipeline-Internship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29DF4013-242A-4DD7-AC3B-F17C03F42D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7293EE80-2CCE-414A-A93D-CF4C4C170742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>Task</t>
   </si>
@@ -257,6 +257,15 @@
   </si>
   <si>
     <t>Tested improved sine sweep v3 with longer duration and extended frequency range. Observed unexpected results. Reverted to v2 and disabled HRTF for mono RIR measurement. Rewrote main_KT Jupyter notebook for modularity. Tested original GDP sweep.wav, noting consistent but low RT60 values. Planned to explore audio source parameter tuning and prepare questions for Dr. Atiyeh.</t>
+  </si>
+  <si>
+    <t>Experimented with reflection mix levels and volume adjustments to address EDT and RT60 issues. Tested normalized sine sweep with lower amplitude. Compared results with Mona's recordings. Implemented volume attenuation in Unity (-10dB to -25dB). Observed persistent high RT60 due to elevated noise floor levels. Identified long reverb tail in RIR time domain graph. Concluded current approaches ineffective in resolving noise floor problem.</t>
+  </si>
+  <si>
+    <t>Created test scenes to isolate Steam Audio issues. Tested empty scene with floor, confirming proper deconvolution but persistent noise floor. Experimented with floorless scene, revealing unexpected small reverb and noise floor. Observed second peak in RIR not reflected in octave band graph. Planned to replicate findings using Mona's code and test on ground truth and S3A project meshes. Initiated research into Unity RIR measurement practices.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tested reflection mix level changes. Prepared questions for Dr. Atiyeh on RIR analysis. Identified and fixed deconvolution method issue. Began rewriting KT Jupyter notebook for compactness and correctness. Experimented with y_fit parameter, noting persistent EDT issues. Planned further testing and refinement for tomorrow.</t>
   </si>
 </sst>
 </file>
@@ -754,7 +763,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -934,7 +943,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="116" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="174" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -944,9 +953,15 @@
       <c r="C9" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
+      <c r="D9" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="6">

</xml_diff>

<commit_message>
tested real sine sweep generated as recorded (got issues prob with inverse filter
</commit_message>
<xml_diff>
--- a/GanttChart.xlsx
+++ b/GanttChart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\AVVR-Pipeline-Internship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7293EE80-2CCE-414A-A93D-CF4C4C170742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{423EBF0D-5667-4F09-8D00-6408BCB79B21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -763,7 +763,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
KT testing on latest main2 script
</commit_message>
<xml_diff>
--- a/GanttChart.xlsx
+++ b/GanttChart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\AVVR-Pipeline-Internship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{423EBF0D-5667-4F09-8D00-6408BCB79B21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53EDFB7-18E3-4626-AE20-3DDE81CD48AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1500" yWindow="1500" windowWidth="17700" windowHeight="9300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="10 Week" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <si>
     <t>Task</t>
   </si>
@@ -266,6 +266,12 @@
   </si>
   <si>
     <t xml:space="preserve"> Tested reflection mix level changes. Prepared questions for Dr. Atiyeh on RIR analysis. Identified and fixed deconvolution method issue. Began rewriting KT Jupyter notebook for compactness and correctness. Experimented with y_fit parameter, noting persistent EDT issues. Planned further testing and refinement for tomorrow.</t>
+  </si>
+  <si>
+    <t>WFH. Reviewed RIR and deconvolution concepts. Searched for Unity projects with realistic RIR simulation. Tested RIR using generated sweep as recorded sweep. Identified potential inverse filter inaccuracy. Explored Audacity plugin for sine sweep and inverse filter generation as alternative to self-generated signals.</t>
+  </si>
+  <si>
+    <t>Met with Dr. Kim. Updated TODO list. Improved sine sweep generation using MATLAB. Enhanced main1_mhby1g21.m script with exponential sweep and noise reduction techniques. Achieved cleaner RIR in sanity checks. Encountered alignment issues in Unity recordings. Tested various volume levels and attenuation settings in KT scene. Identified potential EDT issues. Planned to sync Unity audio recording with player for better alignment.</t>
   </si>
 </sst>
 </file>
@@ -762,8 +768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8289DD30-5B10-44EC-835E-469611DFB1F9}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -963,12 +969,16 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A10" s="6">
         <v>9</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
+      <c r="B10" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>

</xml_diff>

<commit_message>
main2 silence thershold is important to remove noise floor!
</commit_message>
<xml_diff>
--- a/GanttChart.xlsx
+++ b/GanttChart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\AVVR-Pipeline-Internship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53EDFB7-18E3-4626-AE20-3DDE81CD48AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40BD5163-52BB-43FC-BFA2-8FACFE32A785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="1500" windowWidth="17700" windowHeight="9300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
   <si>
     <t>Task</t>
   </si>
@@ -272,6 +272,9 @@
   </si>
   <si>
     <t>Met with Dr. Kim. Updated TODO list. Improved sine sweep generation using MATLAB. Enhanced main1_mhby1g21.m script with exponential sweep and noise reduction techniques. Achieved cleaner RIR in sanity checks. Encountered alignment issues in Unity recordings. Tested various volume levels and attenuation settings in KT scene. Identified potential EDT issues. Planned to sync Unity audio recording with player for better alignment.</t>
+  </si>
+  <si>
+    <t>Synchronized Unity audio recording with player. Modified AudioRecorder.cs and DelayedAudioPlay.cs. Experimented with various preprocessing techniques in main2. Observed inconsistent results across different scenes (KT, LR, open air). Identified issues with EDT consistently higher than RT60. Considered new approach to clean up noise floor in octave bands. Decided to contact Mona for a meeting to discuss findings and persistent issues.</t>
   </si>
 </sst>
 </file>
@@ -768,8 +771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8289DD30-5B10-44EC-835E-469611DFB1F9}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -969,7 +972,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="145" x14ac:dyDescent="0.35">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -979,7 +982,9 @@
       <c r="C10" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D10" s="3"/>
+      <c r="D10" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>

</xml_diff>

<commit_message>
30 sec sine sweep test (not good at all)
</commit_message>
<xml_diff>
--- a/GanttChart.xlsx
+++ b/GanttChart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\AVVR-Pipeline-Internship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40BD5163-52BB-43FC-BFA2-8FACFE32A785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FCDC21C-066A-4DEA-AEC8-A8F498091BE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1500" windowWidth="17700" windowHeight="9300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="10 Week" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
   <si>
     <t>Task</t>
   </si>
@@ -275,6 +275,9 @@
   </si>
   <si>
     <t>Synchronized Unity audio recording with player. Modified AudioRecorder.cs and DelayedAudioPlay.cs. Experimented with various preprocessing techniques in main2. Observed inconsistent results across different scenes (KT, LR, open air). Identified issues with EDT consistently higher than RT60. Considered new approach to clean up noise floor in octave bands. Decided to contact Mona for a meeting to discuss findings and persistent issues.</t>
+  </si>
+  <si>
+    <t>Scheduled meeting with Mona for next Tuesday. Focused on generating results for all scenes for poster preparation. Attempted signal realignment to improve accuracy. Experimented with longer sine sweep (30 sec) to address frequency-dependent RT60/EDT issues. Tested new approach on multiple scenes (KT, LR, ST, UL, MR). Observed persistent inconsistencies in results despite adjustments.</t>
   </si>
 </sst>
 </file>
@@ -636,7 +639,7 @@
   <dimension ref="A1:V8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -734,6 +737,10 @@
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
       <c r="N5" t="s">
         <v>54</v>
       </c>
@@ -771,8 +778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8289DD30-5B10-44EC-835E-469611DFB1F9}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -985,7 +992,9 @@
       <c r="D10" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E10" s="3"/>
+      <c r="E10" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>